<commit_message>
Added tkinter oop version
</commit_message>
<xml_diff>
--- a/ayman_data.xlsx
+++ b/ayman_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\VSCODE\whatsappscript\python_whatsappkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED6B4B2-B332-4C3D-B1A9-DEC6A6BCC720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="14115" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="14115" tabRatio="500" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -55,11 +50,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans Arabic UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -87,18 +88,124 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -406,14 +513,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.504999999999999" defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
@@ -440,294 +547,295 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1281526570</v>
+        <v>1204086820</v>
       </c>
       <c r="D2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3">
+    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1281526570</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D3" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
-      <c r="A4">
+    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>1281526570</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D4" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5">
+    <row r="5" spans="1:4" ht="15" customHeight="1">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>1281526570</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D5" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="A6">
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>1281526570</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D6" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="A7">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>1281526570</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D7" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>1281526570</v>
-      </c>
-      <c r="D8">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D8" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9">
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>1281526570</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D9" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10">
+    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>1281526570</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D10" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
-      <c r="A11">
+    <row r="11" spans="1:4" ht="15" customHeight="1">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>1281526570</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D11" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
-      <c r="A12">
+    <row r="12" spans="1:4" ht="15" customHeight="1">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>1281526570</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D12" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
-      <c r="A13">
+    <row r="13" spans="1:4" ht="15" customHeight="1">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13">
-        <v>1281526570</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D13" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
-      <c r="A14">
+    <row r="14" spans="1:4" ht="15" customHeight="1">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>1281526570</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D14" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
-      <c r="A15">
+    <row r="15" spans="1:4" ht="15" customHeight="1">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>1281526570</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D15" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
-      <c r="A16">
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>1281526570</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D16" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
-      <c r="A17">
+    <row r="17" spans="1:4" ht="15" customHeight="1">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>1281526570</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D17" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="A18">
+    <row r="18" spans="1:4" ht="15" customHeight="1">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>1281526570</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D18" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
-      <c r="A19">
+    <row r="19" spans="1:4" ht="15" customHeight="1">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>1281526570</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D19" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
-      <c r="A20">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>1281526570</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D20" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="A21">
+    <row r="21" spans="1:4" ht="15" customHeight="1">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21">
-        <v>1281526570</v>
-      </c>
-      <c r="D21">
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D21" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
-      <c r="A22">
+    <row r="22" spans="1:4" ht="15" customHeight="1">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>1281526570</v>
-      </c>
-      <c r="D22">
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1204086820</v>
+      </c>
+      <c r="D22" s="2">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>